<commit_message>
updaing with 4ha and greater lakes
</commit_message>
<xml_diff>
--- a/Copy of criteria_thresholds.xlsx
+++ b/Copy of criteria_thresholds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Downloads\PhD_code\STOICH_NARSchallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEA41000-ADA8-4CD0-B9B6-81287AFEC96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B74836A-079F-4957-AE45-40031A30F4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{214A31F5-56E4-480B-8EF3-6EDB9B7AF7F5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{214A31F5-56E4-480B-8EF3-6EDB9B7AF7F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,20 +87,17 @@
     <t>DIN mg L-1 concentration threshold</t>
   </si>
   <si>
-    <t>Average DIN:TP molar ratio</t>
-  </si>
-  <si>
     <t>Average TN:TP molar ratio</t>
+  </si>
+  <si>
+    <t>Median DIN:TP molar ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +119,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +138,11 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -208,18 +217,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -229,8 +235,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,7 +568,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,53 +576,55 @@
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10" style="13" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="13" customWidth="1"/>
     <col min="6" max="6" width="10.109375" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="10.88671875" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" customWidth="1"/>
     <col min="10" max="11" width="10.44140625" customWidth="1"/>
+    <col min="12" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="11" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="11" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="11" t="s">
+      <c r="M1" s="8"/>
+      <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="11" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="12"/>
+      <c r="Q1" s="8"/>
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
@@ -609,10 +633,10 @@
       <c r="C2" s="3">
         <v>2017</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="11">
         <v>2007</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="12">
         <v>2017</v>
       </c>
       <c r="F2" s="2">
@@ -654,434 +678,434 @@
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
-        <v>21.5367954422595</v>
-      </c>
-      <c r="C3" s="5">
-        <v>3.9920002674388702</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="B3" s="15">
+        <v>5.3439893026225</v>
+      </c>
+      <c r="C3" s="15">
+        <v>2.07893500059392</v>
+      </c>
+      <c r="D3" s="16">
         <v>108.48881317764101</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="17">
         <v>62.615709803804599</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="15">
         <v>0.01</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="15">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="15">
         <v>2.4E-2</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="15">
         <v>1.06E-2</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="15">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="15">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="L3" s="4">
-        <v>4.75</v>
-      </c>
-      <c r="M3" s="5">
-        <v>8.1587499999999995</v>
-      </c>
-      <c r="N3" s="4">
+      <c r="L3" s="15">
+        <v>4.625</v>
+      </c>
+      <c r="M3" s="15">
+        <v>7.9965624999999996</v>
+      </c>
+      <c r="N3" s="15">
         <v>11</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="15">
         <v>13.6621875</v>
       </c>
-      <c r="P3" s="4">
-        <v>7.875</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>10.91046875</v>
+      <c r="P3" s="15">
+        <v>7.8125</v>
+      </c>
+      <c r="Q3" s="15">
+        <v>10.829375000000001</v>
       </c>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
-        <v>38.073158823868397</v>
-      </c>
-      <c r="C4" s="5">
-        <v>14.138287600291299</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="B4" s="15">
+        <v>3.1822960170789099</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1.78885979702832</v>
+      </c>
+      <c r="D4" s="16">
         <v>96.356019020985798</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="17">
         <v>61.837008113890001</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="15">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G4" s="15">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H4" s="15">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I4" s="15">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="J4" s="15">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K4" s="15">
+        <v>7.7499999999999999E-3</v>
+      </c>
+      <c r="L4" s="15">
+        <v>7</v>
+      </c>
+      <c r="M4" s="15">
+        <v>9.5693750000000009</v>
+      </c>
+      <c r="N4" s="15">
+        <v>10</v>
+      </c>
+      <c r="O4" s="15">
+        <v>16.374375000000001</v>
+      </c>
+      <c r="P4" s="15">
+        <v>8.5</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>12.971875000000001</v>
+      </c>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15">
+        <v>1.17936315644082</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0.73686579784031203</v>
+      </c>
+      <c r="D5" s="16">
+        <v>43.776446031888</v>
+      </c>
+      <c r="E5" s="17">
+        <v>46.170842511033797</v>
+      </c>
+      <c r="F5" s="15">
+        <v>1.6250000000000001E-2</v>
+      </c>
+      <c r="G5" s="15">
         <v>0.01</v>
       </c>
-      <c r="G4" s="5">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="H4" s="4">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="I4" s="5">
-        <v>8.5000000000000006E-3</v>
-      </c>
-      <c r="J4" s="4">
-        <v>1.6E-2</v>
-      </c>
-      <c r="K4" s="5">
-        <v>7.7499999999999999E-3</v>
-      </c>
-      <c r="L4" s="4">
-        <v>7.375</v>
-      </c>
-      <c r="M4" s="5">
-        <v>9.9353125000000002</v>
-      </c>
-      <c r="N4" s="4">
-        <v>10</v>
-      </c>
-      <c r="O4" s="5">
-        <v>16.374375000000001</v>
-      </c>
-      <c r="P4" s="4">
-        <v>8.6875</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>13.15484375</v>
-      </c>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>4.4180728027305296</v>
-      </c>
-      <c r="C5" s="5">
-        <v>5.9004088622114503</v>
-      </c>
-      <c r="D5" s="4">
-        <v>43.776446031888</v>
-      </c>
-      <c r="E5" s="5">
-        <v>46.170842511033797</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1.6625000000000001E-2</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="H5" s="15">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="15">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="J5" s="4">
-        <v>1.7312500000000001E-2</v>
-      </c>
-      <c r="K5" s="5">
+      <c r="J5" s="15">
+        <v>1.7125000000000001E-2</v>
+      </c>
+      <c r="K5" s="15">
         <v>1.15E-2</v>
       </c>
-      <c r="L5" s="4">
-        <v>28.25</v>
-      </c>
-      <c r="M5" s="5">
-        <v>24.61045</v>
-      </c>
-      <c r="N5" s="4">
+      <c r="L5" s="15">
+        <v>28.5</v>
+      </c>
+      <c r="M5" s="15">
+        <v>24.727150000000002</v>
+      </c>
+      <c r="N5" s="15">
         <v>36</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="15">
         <v>24.727150000000002</v>
       </c>
-      <c r="P5" s="4">
-        <v>32.125</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>24.668800000000001</v>
+      <c r="P5" s="15">
+        <v>32.25</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>24.727150000000002</v>
       </c>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>6.3408043761810697</v>
-      </c>
-      <c r="C6" s="5">
-        <v>6.6728954847139796</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="B6" s="15">
+        <v>1.15590991185252</v>
+      </c>
+      <c r="C6" s="15">
+        <v>1.0300734362548301</v>
+      </c>
+      <c r="D6" s="16">
         <v>46.143855143962398</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="17">
         <v>46.362506658605099</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="15">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G6" s="5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="G6" s="15">
+        <v>1.5225000000000001E-2</v>
+      </c>
+      <c r="H6" s="15">
         <v>0.13775000000000001</v>
       </c>
-      <c r="I6" s="5">
-        <v>3.1774999999999998E-2</v>
-      </c>
-      <c r="J6" s="4">
+      <c r="I6" s="15">
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="J6" s="15">
         <v>7.9375000000000001E-2</v>
       </c>
-      <c r="K6" s="5">
-        <v>2.3387499999999999E-2</v>
-      </c>
-      <c r="L6" s="4">
-        <v>33.75</v>
-      </c>
-      <c r="M6" s="5">
-        <v>35.147500000000001</v>
-      </c>
-      <c r="N6" s="4">
+      <c r="K6" s="15">
+        <v>1.8662499999999999E-2</v>
+      </c>
+      <c r="L6" s="15">
+        <v>33</v>
+      </c>
+      <c r="M6" s="15">
+        <v>35.1</v>
+      </c>
+      <c r="N6" s="15">
         <v>80.5</v>
       </c>
-      <c r="O6" s="5">
-        <v>49.745624999999997</v>
-      </c>
-      <c r="P6" s="4">
-        <v>57.125</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>42.446562499999999</v>
+      <c r="O6" s="15">
+        <v>46.309375000000003</v>
+      </c>
+      <c r="P6" s="15">
+        <v>56.75</v>
+      </c>
+      <c r="Q6" s="15">
+        <v>40.704687499999999</v>
       </c>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
-        <v>17.808863731669799</v>
-      </c>
-      <c r="C7" s="5">
-        <v>13.833012886828399</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="B7" s="15">
+        <v>4.4226118366530898</v>
+      </c>
+      <c r="C7" s="15">
+        <v>2.1446557064546798</v>
+      </c>
+      <c r="D7" s="16">
         <v>132.49660732721199</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="17">
         <v>88.940704351994697</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="15">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="15">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="15">
         <v>3.9E-2</v>
       </c>
-      <c r="I7" s="5">
-        <v>0.63619999999999999</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="I7" s="15">
+        <v>0.64922500000000005</v>
+      </c>
+      <c r="J7" s="15">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="K7" s="5">
-        <v>0.3236</v>
-      </c>
-      <c r="L7" s="4">
+      <c r="K7" s="15">
+        <v>0.33011249999999998</v>
+      </c>
+      <c r="L7" s="15">
         <v>8</v>
       </c>
-      <c r="M7" s="5">
-        <v>13.3725</v>
-      </c>
-      <c r="N7" s="4">
+      <c r="M7" s="15">
+        <v>12.719374999999999</v>
+      </c>
+      <c r="N7" s="15">
         <v>9.5</v>
       </c>
-      <c r="O7" s="5">
-        <v>33.353749999999998</v>
-      </c>
-      <c r="P7" s="4">
+      <c r="O7" s="15">
+        <v>40.586562499999999</v>
+      </c>
+      <c r="P7" s="15">
         <v>8.75</v>
       </c>
-      <c r="Q7" s="5">
-        <v>23.363125</v>
+      <c r="Q7" s="15">
+        <v>26.652968749999999</v>
       </c>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
-        <v>4.4322867835876298</v>
-      </c>
-      <c r="C8" s="5">
-        <v>23.886035555890199</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="B8" s="15">
+        <v>1.66571268240299</v>
+      </c>
+      <c r="C8" s="15">
+        <v>1.0833432993960099</v>
+      </c>
+      <c r="D8" s="16">
         <v>48.857926238166598</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="17">
         <v>67.017227853136404</v>
       </c>
-      <c r="F8" s="4">
-        <v>4.2750000000000003E-2</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1.9449999999999999E-2</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="F8" s="15">
+        <v>3.95E-2</v>
+      </c>
+      <c r="G8" s="15">
+        <v>1.9425000000000001E-2</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="J8" s="4">
-        <v>4.2750000000000003E-2</v>
-      </c>
-      <c r="K8" s="5">
-        <v>2.9725000000000001E-2</v>
-      </c>
-      <c r="L8" s="4">
+      <c r="I8" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="J8" s="15">
+        <v>3.95E-2</v>
+      </c>
+      <c r="K8" s="15">
+        <v>2.4712499999999998E-2</v>
+      </c>
+      <c r="L8" s="15">
         <v>61</v>
       </c>
-      <c r="M8" s="5">
-        <v>48.220624999999998</v>
-      </c>
-      <c r="N8" s="4" t="s">
+      <c r="M8" s="15">
+        <v>40.378937499999999</v>
+      </c>
+      <c r="N8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="5">
-        <v>275.62374999999997</v>
-      </c>
-      <c r="P8" s="4">
+      <c r="O8" s="15">
+        <v>161.16999999999999</v>
+      </c>
+      <c r="P8" s="15">
         <v>61</v>
       </c>
-      <c r="Q8" s="5">
-        <v>161.92218750000001</v>
+      <c r="Q8" s="15">
+        <v>100.77446875</v>
       </c>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
-        <v>3.6076121034641901</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1.9897927877125701</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="B9" s="15">
+        <v>1.61899183306051</v>
+      </c>
+      <c r="C9" s="15">
+        <v>0.98019966131472802</v>
+      </c>
+      <c r="D9" s="16">
         <v>41.368667396810601</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="17">
         <v>37.894391845330503</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="15">
         <v>1.9E-2</v>
       </c>
-      <c r="G9" s="5">
-        <v>1.23E-2</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="G9" s="15">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H9" s="15">
         <v>6.3250000000000001E-2</v>
       </c>
-      <c r="I9" s="5">
-        <v>6.4500000000000002E-2</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="I9" s="15">
+        <v>6.1600000000000002E-2</v>
+      </c>
+      <c r="J9" s="15">
         <v>4.1125000000000002E-2</v>
       </c>
-      <c r="K9" s="5">
-        <v>3.8399999999999997E-2</v>
-      </c>
-      <c r="L9" s="4">
+      <c r="K9" s="15">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="L9" s="15">
         <v>24</v>
       </c>
-      <c r="M9" s="5">
-        <v>25.887812499999999</v>
-      </c>
-      <c r="N9" s="4">
+      <c r="M9" s="15">
+        <v>23.594999999999999</v>
+      </c>
+      <c r="N9" s="15">
         <v>533.75</v>
       </c>
-      <c r="O9" s="5">
-        <v>55.117812499999999</v>
-      </c>
-      <c r="P9" s="4">
+      <c r="O9" s="15">
+        <v>48.684375000000003</v>
+      </c>
+      <c r="P9" s="15">
         <v>278.875</v>
       </c>
-      <c r="Q9" s="5">
-        <v>40.502812499999997</v>
+      <c r="Q9" s="15">
+        <v>36.139687500000001</v>
       </c>
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
-        <v>29.0534733648837</v>
-      </c>
-      <c r="C10" s="5">
-        <v>6.4460726567717597</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="B10" s="15">
+        <v>2.4352715177467998</v>
+      </c>
+      <c r="C10" s="15">
+        <v>1.4586180573920999</v>
+      </c>
+      <c r="D10" s="16">
         <v>78.379918845240994</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="17">
         <v>43.605191057508698</v>
       </c>
-      <c r="F10" s="4">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="G10" s="5">
+      <c r="F10" s="15">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="G10" s="15">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="15">
         <v>1.525E-2</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="15">
         <v>1.5900000000000001E-2</v>
       </c>
-      <c r="J10" s="4">
-        <v>1.6625000000000001E-2</v>
-      </c>
-      <c r="K10" s="5">
+      <c r="J10" s="15">
+        <v>1.6375000000000001E-2</v>
+      </c>
+      <c r="K10" s="15">
         <v>1.4449999999999999E-2</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="15">
         <v>15</v>
       </c>
-      <c r="M10" s="5">
-        <v>19.094999999999999</v>
-      </c>
-      <c r="N10" s="4">
+      <c r="M10" s="15">
+        <v>17.81625</v>
+      </c>
+      <c r="N10" s="15">
         <v>48.25</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="15">
         <v>21.506562500000001</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="15">
         <v>31.625</v>
       </c>
-      <c r="Q10" s="5">
-        <v>20.30078125</v>
+      <c r="Q10" s="15">
+        <v>19.661406249999999</v>
       </c>
       <c r="R10" s="1"/>
     </row>
@@ -1089,53 +1113,53 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="6">
-        <v>15.162589210678201</v>
-      </c>
-      <c r="C11" s="7">
-        <v>4.3753228399387103</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="B11" s="15">
+        <v>3.93121052146943</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1.49236100443836</v>
+      </c>
+      <c r="D11" s="18">
         <v>71.695289350395598</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="19">
         <v>44.220981492436003</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="15">
         <v>0.01</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="15">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="15">
         <v>0.01</v>
       </c>
-      <c r="I11" s="7">
-        <v>1.6449999999999999E-2</v>
-      </c>
-      <c r="J11" s="6">
+      <c r="I11" s="15">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="J11" s="15">
         <v>0.01</v>
       </c>
-      <c r="K11" s="7">
-        <v>1.2225E-2</v>
-      </c>
-      <c r="L11" s="6">
+      <c r="K11" s="15">
+        <v>1.2449999999999999E-2</v>
+      </c>
+      <c r="L11" s="15">
         <v>4</v>
       </c>
-      <c r="M11" s="7">
-        <v>9.5956250000000001</v>
-      </c>
-      <c r="N11" s="6">
+      <c r="M11" s="15">
+        <v>8.7912499999999998</v>
+      </c>
+      <c r="N11" s="15">
         <v>4</v>
       </c>
-      <c r="O11" s="7">
-        <v>14.0665625</v>
-      </c>
-      <c r="P11" s="6">
+      <c r="O11" s="15">
+        <v>14.701874999999999</v>
+      </c>
+      <c r="P11" s="15">
         <v>4</v>
       </c>
-      <c r="Q11" s="7">
-        <v>11.831093750000001</v>
+      <c r="Q11" s="15">
+        <v>11.7465625</v>
       </c>
       <c r="R11" s="1"/>
     </row>
@@ -1157,7 +1181,7 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1175,7 +1199,7 @@
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1193,7 +1217,7 @@
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1211,7 +1235,7 @@
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>

</xml_diff>